<commit_message>
DP: create_forecast_basic - fututre - palestinian_from_demo_230622.ipynb - make dynamic & compare
</commit_message>
<xml_diff>
--- a/create_forecast_basic/future/arab_and_palestinian/Intermediates/taz_demo_pls_2020_and_pre_growth_till_2050.xlsx
+++ b/create_forecast_basic/future/arab_and_palestinian/Intermediates/taz_demo_pls_2020_and_pre_growth_till_2050.xlsx
@@ -480,7 +480,7 @@
         <v>3608</v>
       </c>
       <c r="B2" t="n">
-        <v>1056.376143503586</v>
+        <v>1056.376143503587</v>
       </c>
       <c r="C2" t="n">
         <v>1.09</v>
@@ -506,7 +506,7 @@
         <v>7043</v>
       </c>
       <c r="B3" t="n">
-        <v>3351.030090095652</v>
+        <v>3351.030090095651</v>
       </c>
       <c r="C3" t="n">
         <v>1.07</v>
@@ -532,7 +532,7 @@
         <v>7101</v>
       </c>
       <c r="B4" t="n">
-        <v>2962.840831427094</v>
+        <v>2962.840831427092</v>
       </c>
       <c r="C4" t="n">
         <v>1.07</v>
@@ -558,7 +558,7 @@
         <v>7102</v>
       </c>
       <c r="B5" t="n">
-        <v>13657.09255956938</v>
+        <v>13657.09255956939</v>
       </c>
       <c r="C5" t="n">
         <v>1.07</v>
@@ -610,7 +610,7 @@
         <v>7104</v>
       </c>
       <c r="B7" t="n">
-        <v>7745.569440416215</v>
+        <v>7745.569440416222</v>
       </c>
       <c r="C7" t="n">
         <v>1.07</v>
@@ -688,7 +688,7 @@
         <v>7222</v>
       </c>
       <c r="B10" t="n">
-        <v>12947.46957820609</v>
+        <v>12947.46957820608</v>
       </c>
       <c r="C10" t="n">
         <v>1.09</v>
@@ -714,7 +714,7 @@
         <v>7223</v>
       </c>
       <c r="B11" t="n">
-        <v>8352.922973942597</v>
+        <v>8352.922973942599</v>
       </c>
       <c r="C11" t="n">
         <v>1.09</v>
@@ -740,7 +740,7 @@
         <v>7231</v>
       </c>
       <c r="B12" t="n">
-        <v>31534.82207316571</v>
+        <v>31534.82207316569</v>
       </c>
       <c r="C12" t="n">
         <v>1.11</v>
@@ -792,7 +792,7 @@
         <v>7233</v>
       </c>
       <c r="B14" t="n">
-        <v>23312.40407293032</v>
+        <v>23312.40407293034</v>
       </c>
       <c r="C14" t="n">
         <v>1.11</v>
@@ -818,7 +818,7 @@
         <v>7240</v>
       </c>
       <c r="B15" t="n">
-        <v>9238.337304094544</v>
+        <v>9238.337304094539</v>
       </c>
       <c r="C15" t="n">
         <v>1.07</v>
@@ -844,7 +844,7 @@
         <v>7241</v>
       </c>
       <c r="B16" t="n">
-        <v>1356.859296695618</v>
+        <v>1356.859296695617</v>
       </c>
       <c r="C16" t="n">
         <v>1.07</v>
@@ -870,7 +870,7 @@
         <v>7242</v>
       </c>
       <c r="B17" t="n">
-        <v>6647.841362719091</v>
+        <v>6647.841362719089</v>
       </c>
       <c r="C17" t="n">
         <v>1.07</v>
@@ -896,7 +896,7 @@
         <v>7243</v>
       </c>
       <c r="B18" t="n">
-        <v>2312.506257157636</v>
+        <v>2312.506257157635</v>
       </c>
       <c r="C18" t="n">
         <v>1.07</v>
@@ -922,7 +922,7 @@
         <v>7244</v>
       </c>
       <c r="B19" t="n">
-        <v>2097.365229891026</v>
+        <v>2097.365229891025</v>
       </c>
       <c r="C19" t="n">
         <v>1.07</v>
@@ -948,7 +948,7 @@
         <v>7245</v>
       </c>
       <c r="B20" t="n">
-        <v>11984.16119587551</v>
+        <v>11984.16119587552</v>
       </c>
       <c r="C20" t="n">
         <v>1.07</v>
@@ -1000,7 +1000,7 @@
         <v>7247</v>
       </c>
       <c r="B22" t="n">
-        <v>9259.720527079418</v>
+        <v>9259.720527079417</v>
       </c>
       <c r="C22" t="n">
         <v>1.07</v>
@@ -1078,7 +1078,7 @@
         <v>7250</v>
       </c>
       <c r="B25" t="n">
-        <v>2826.269083827389</v>
+        <v>2826.26908382739</v>
       </c>
       <c r="C25" t="n">
         <v>1.07</v>
@@ -1104,7 +1104,7 @@
         <v>7251</v>
       </c>
       <c r="B26" t="n">
-        <v>7018.426027331157</v>
+        <v>7018.426027331168</v>
       </c>
       <c r="C26" t="n">
         <v>1.07</v>
@@ -1156,7 +1156,7 @@
         <v>7253</v>
       </c>
       <c r="B28" t="n">
-        <v>6474.571007564195</v>
+        <v>6474.571007564197</v>
       </c>
       <c r="C28" t="n">
         <v>1.07</v>
@@ -1260,7 +1260,7 @@
         <v>7911</v>
       </c>
       <c r="B32" t="n">
-        <v>31438.22357473389</v>
+        <v>31438.22357473388</v>
       </c>
       <c r="C32" t="n">
         <v>1.08</v>
@@ -1286,7 +1286,7 @@
         <v>7912</v>
       </c>
       <c r="B33" t="n">
-        <v>8400.779393415714</v>
+        <v>8400.779393415709</v>
       </c>
       <c r="C33" t="n">
         <v>1.08</v>
@@ -1312,7 +1312,7 @@
         <v>7913</v>
       </c>
       <c r="B34" t="n">
-        <v>10616.04829648282</v>
+        <v>10616.04829648283</v>
       </c>
       <c r="C34" t="n">
         <v>1.08</v>
@@ -1338,7 +1338,7 @@
         <v>7921</v>
       </c>
       <c r="B35" t="n">
-        <v>22800.34041347285</v>
+        <v>22800.34041347284</v>
       </c>
       <c r="C35" t="n">
         <v>1.08</v>
@@ -1416,7 +1416,7 @@
         <v>7931</v>
       </c>
       <c r="B38" t="n">
-        <v>5503.540562500063</v>
+        <v>5503.540562500059</v>
       </c>
       <c r="C38" t="n">
         <v>1.07</v>
@@ -1442,7 +1442,7 @@
         <v>7932</v>
       </c>
       <c r="B39" t="n">
-        <v>4638.438260132138</v>
+        <v>4638.438260132139</v>
       </c>
       <c r="C39" t="n">
         <v>1.07</v>
@@ -1520,7 +1520,7 @@
         <v>7935</v>
       </c>
       <c r="B42" t="n">
-        <v>3639.868562663517</v>
+        <v>3639.868562663518</v>
       </c>
       <c r="C42" t="n">
         <v>1.07</v>
@@ -1546,7 +1546,7 @@
         <v>7936</v>
       </c>
       <c r="B43" t="n">
-        <v>574.8988494540239</v>
+        <v>574.8988494540241</v>
       </c>
       <c r="C43" t="n">
         <v>1.07</v>
@@ -1676,7 +1676,7 @@
         <v>7941</v>
       </c>
       <c r="B48" t="n">
-        <v>3282.349193585458</v>
+        <v>3282.349193585456</v>
       </c>
       <c r="C48" t="n">
         <v>1.07</v>
@@ -1754,7 +1754,7 @@
         <v>7944</v>
       </c>
       <c r="B51" t="n">
-        <v>2159.886225478472</v>
+        <v>2159.886225478473</v>
       </c>
       <c r="C51" t="n">
         <v>1.07</v>
@@ -1988,7 +1988,7 @@
         <v>7953</v>
       </c>
       <c r="B60" t="n">
-        <v>3665.597929885506</v>
+        <v>3665.597929885505</v>
       </c>
       <c r="C60" t="n">
         <v>1.07</v>
@@ -2014,7 +2014,7 @@
         <v>7954</v>
       </c>
       <c r="B61" t="n">
-        <v>6208.064626217226</v>
+        <v>6208.064626217228</v>
       </c>
       <c r="C61" t="n">
         <v>1.07</v>
@@ -2040,7 +2040,7 @@
         <v>7955</v>
       </c>
       <c r="B62" t="n">
-        <v>3075.2020213341</v>
+        <v>3075.202021334099</v>
       </c>
       <c r="C62" t="n">
         <v>1.07</v>
@@ -2144,7 +2144,7 @@
         <v>7961</v>
       </c>
       <c r="B66" t="n">
-        <v>2460.597893549262</v>
+        <v>2460.597893549263</v>
       </c>
       <c r="C66" t="n">
         <v>1.07</v>
@@ -2170,7 +2170,7 @@
         <v>7962</v>
       </c>
       <c r="B67" t="n">
-        <v>3811.739749734853</v>
+        <v>3811.739749734852</v>
       </c>
       <c r="C67" t="n">
         <v>1.07</v>
@@ -2222,7 +2222,7 @@
         <v>7964</v>
       </c>
       <c r="B69" t="n">
-        <v>4262.668554997998</v>
+        <v>4262.668554997999</v>
       </c>
       <c r="C69" t="n">
         <v>1.07</v>
@@ -2248,7 +2248,7 @@
         <v>7965</v>
       </c>
       <c r="B70" t="n">
-        <v>4891.570341387478</v>
+        <v>4891.570341387477</v>
       </c>
       <c r="C70" t="n">
         <v>1.07</v>
@@ -2300,7 +2300,7 @@
         <v>7967</v>
       </c>
       <c r="B72" t="n">
-        <v>7247.22757881587</v>
+        <v>7247.227578815873</v>
       </c>
       <c r="C72" t="n">
         <v>1.07</v>
@@ -2326,7 +2326,7 @@
         <v>7968</v>
       </c>
       <c r="B73" t="n">
-        <v>5075.153552924234</v>
+        <v>5075.153552924236</v>
       </c>
       <c r="C73" t="n">
         <v>1.07</v>
@@ -2352,7 +2352,7 @@
         <v>7969</v>
       </c>
       <c r="B74" t="n">
-        <v>6347.776266459361</v>
+        <v>6347.776266459362</v>
       </c>
       <c r="C74" t="n">
         <v>1.07</v>
@@ -2378,7 +2378,7 @@
         <v>8211</v>
       </c>
       <c r="B75" t="n">
-        <v>38560.82244730266</v>
+        <v>38560.82244730265</v>
       </c>
       <c r="C75" t="n">
         <v>1.12</v>
@@ -2404,7 +2404,7 @@
         <v>8212</v>
       </c>
       <c r="B76" t="n">
-        <v>33424.25640304456</v>
+        <v>33424.25640304457</v>
       </c>
       <c r="C76" t="n">
         <v>1.12</v>
@@ -2430,7 +2430,7 @@
         <v>8221</v>
       </c>
       <c r="B77" t="n">
-        <v>37700.44052765586</v>
+        <v>37700.44052765588</v>
       </c>
       <c r="C77" t="n">
         <v>1.11</v>
@@ -2456,7 +2456,7 @@
         <v>8222</v>
       </c>
       <c r="B78" t="n">
-        <v>40311.11348836826</v>
+        <v>40311.11348836825</v>
       </c>
       <c r="C78" t="n">
         <v>1.11</v>
@@ -2482,7 +2482,7 @@
         <v>8223</v>
       </c>
       <c r="B79" t="n">
-        <v>49008.68950588788</v>
+        <v>49008.68950588787</v>
       </c>
       <c r="C79" t="n">
         <v>1.11</v>
@@ -2508,7 +2508,7 @@
         <v>8224</v>
       </c>
       <c r="B80" t="n">
-        <v>61819.98505985027</v>
+        <v>61819.98505985031</v>
       </c>
       <c r="C80" t="n">
         <v>1.11</v>
@@ -2534,7 +2534,7 @@
         <v>8225</v>
       </c>
       <c r="B81" t="n">
-        <v>1445.558808736116</v>
+        <v>1445.558808736117</v>
       </c>
       <c r="C81" t="n">
         <v>1.09</v>
@@ -2560,7 +2560,7 @@
         <v>8230</v>
       </c>
       <c r="B82" t="n">
-        <v>10710.75837283999</v>
+        <v>10710.75837284</v>
       </c>
       <c r="C82" t="n">
         <v>1.12</v>
@@ -2690,7 +2690,7 @@
         <v>8236</v>
       </c>
       <c r="B87" t="n">
-        <v>6334.876780489883</v>
+        <v>6334.876780489882</v>
       </c>
       <c r="C87" t="n">
         <v>1.12</v>
@@ -2768,7 +2768,7 @@
         <v>8241</v>
       </c>
       <c r="B90" t="n">
-        <v>6177.619005787365</v>
+        <v>6177.619005787363</v>
       </c>
       <c r="C90" t="n">
         <v>1.12</v>
@@ -2820,7 +2820,7 @@
         <v>8243</v>
       </c>
       <c r="B92" t="n">
-        <v>2322.229844352049</v>
+        <v>2322.22984435205</v>
       </c>
       <c r="C92" t="n">
         <v>1.12</v>
@@ -2846,7 +2846,7 @@
         <v>8244</v>
       </c>
       <c r="B93" t="n">
-        <v>3072.386451623352</v>
+        <v>3072.386451623351</v>
       </c>
       <c r="C93" t="n">
         <v>1.12</v>
@@ -2924,7 +2924,7 @@
         <v>8247</v>
       </c>
       <c r="B96" t="n">
-        <v>7820.075338082473</v>
+        <v>7820.075338082474</v>
       </c>
       <c r="C96" t="n">
         <v>1.12</v>
@@ -2950,7 +2950,7 @@
         <v>8248</v>
       </c>
       <c r="B97" t="n">
-        <v>10102.33349422885</v>
+        <v>10102.33349422886</v>
       </c>
       <c r="C97" t="n">
         <v>1.12</v>
@@ -3028,7 +3028,7 @@
         <v>8251</v>
       </c>
       <c r="B100" t="n">
-        <v>3643.475270651657</v>
+        <v>3643.475270651656</v>
       </c>
       <c r="C100" t="n">
         <v>1.12</v>
@@ -3080,7 +3080,7 @@
         <v>8253</v>
       </c>
       <c r="B102" t="n">
-        <v>19767.59212547422</v>
+        <v>19767.59212547423</v>
       </c>
       <c r="C102" t="n">
         <v>1.12</v>
@@ -3158,7 +3158,7 @@
         <v>8256</v>
       </c>
       <c r="B105" t="n">
-        <v>12177.0473042112</v>
+        <v>12177.04730421119</v>
       </c>
       <c r="C105" t="n">
         <v>1.12</v>
@@ -3184,7 +3184,7 @@
         <v>8261</v>
       </c>
       <c r="B106" t="n">
-        <v>51759.29083614592</v>
+        <v>51759.29083614588</v>
       </c>
       <c r="C106" t="n">
         <v>1.11</v>
@@ -3340,7 +3340,7 @@
         <v>8722</v>
       </c>
       <c r="B112" t="n">
-        <v>10117.36000725107</v>
+        <v>10117.36000725108</v>
       </c>
       <c r="C112" t="n">
         <v>1.08</v>
@@ -3366,7 +3366,7 @@
         <v>8723</v>
       </c>
       <c r="B113" t="n">
-        <v>8137.56778567266</v>
+        <v>8137.567785672659</v>
       </c>
       <c r="C113" t="n">
         <v>1.08</v>
@@ -3392,7 +3392,7 @@
         <v>8724</v>
       </c>
       <c r="B114" t="n">
-        <v>18893.69111760744</v>
+        <v>18893.69111760743</v>
       </c>
       <c r="C114" t="n">
         <v>1.08</v>
@@ -3418,7 +3418,7 @@
         <v>8731</v>
       </c>
       <c r="B115" t="n">
-        <v>23016.59333840669</v>
+        <v>23016.5933384067</v>
       </c>
       <c r="C115" t="n">
         <v>1.09</v>
@@ -3444,7 +3444,7 @@
         <v>8732</v>
       </c>
       <c r="B116" t="n">
-        <v>32210.05347386873</v>
+        <v>32210.05347386872</v>
       </c>
       <c r="C116" t="n">
         <v>1.09</v>
@@ -3522,7 +3522,7 @@
         <v>8743</v>
       </c>
       <c r="B119" t="n">
-        <v>6903.624101767427</v>
+        <v>6903.624101767426</v>
       </c>
       <c r="C119" t="n">
         <v>1.08</v>
@@ -3548,7 +3548,7 @@
         <v>8744</v>
       </c>
       <c r="B120" t="n">
-        <v>8294.373116137094</v>
+        <v>8294.373116137092</v>
       </c>
       <c r="C120" t="n">
         <v>1.08</v>
@@ -3574,7 +3574,7 @@
         <v>8745</v>
       </c>
       <c r="B121" t="n">
-        <v>5510.71596450443</v>
+        <v>5510.715964504432</v>
       </c>
       <c r="C121" t="n">
         <v>1.08</v>
@@ -3600,7 +3600,7 @@
         <v>8911</v>
       </c>
       <c r="B122" t="n">
-        <v>2833.033328839333</v>
+        <v>2833.033328839332</v>
       </c>
       <c r="C122" t="n">
         <v>1.09</v>
@@ -3652,7 +3652,7 @@
         <v>8913</v>
       </c>
       <c r="B124" t="n">
-        <v>8567.557798070324</v>
+        <v>8567.557798070326</v>
       </c>
       <c r="C124" t="n">
         <v>1.09</v>
@@ -3678,7 +3678,7 @@
         <v>8914</v>
       </c>
       <c r="B125" t="n">
-        <v>3197.067857085175</v>
+        <v>3197.067857085174</v>
       </c>
       <c r="C125" t="n">
         <v>1.09</v>
@@ -3704,7 +3704,7 @@
         <v>8921</v>
       </c>
       <c r="B126" t="n">
-        <v>3957.296797336277</v>
+        <v>3957.296797336278</v>
       </c>
       <c r="C126" t="n">
         <v>1.08</v>
@@ -3756,7 +3756,7 @@
         <v>8923</v>
       </c>
       <c r="B128" t="n">
-        <v>8496.015383332367</v>
+        <v>8496.015383332371</v>
       </c>
       <c r="C128" t="n">
         <v>1.09</v>
@@ -3782,7 +3782,7 @@
         <v>8924</v>
       </c>
       <c r="B129" t="n">
-        <v>9740.279703892998</v>
+        <v>9740.279703892995</v>
       </c>
       <c r="C129" t="n">
         <v>1.09</v>
@@ -3964,7 +3964,7 @@
         <v>8951</v>
       </c>
       <c r="B136" t="n">
-        <v>6947.40423989866</v>
+        <v>6947.404239898661</v>
       </c>
       <c r="C136" t="n">
         <v>1.11</v>
@@ -3990,7 +3990,7 @@
         <v>8952</v>
       </c>
       <c r="B137" t="n">
-        <v>63147.65753054974</v>
+        <v>63147.65753054975</v>
       </c>
       <c r="C137" t="n">
         <v>1.11</v>
@@ -4146,7 +4146,7 @@
         <v>8961</v>
       </c>
       <c r="B143" t="n">
-        <v>10900.34095406339</v>
+        <v>10900.3409540634</v>
       </c>
       <c r="C143" t="n">
         <v>1.07</v>
@@ -4276,7 +4276,7 @@
         <v>8966</v>
       </c>
       <c r="B148" t="n">
-        <v>5789.7147748713</v>
+        <v>5789.714774871302</v>
       </c>
       <c r="C148" t="n">
         <v>1.09</v>
@@ -4302,7 +4302,7 @@
         <v>8970</v>
       </c>
       <c r="B149" t="n">
-        <v>35620.44781993151</v>
+        <v>35620.44781993152</v>
       </c>
       <c r="C149" t="n">
         <v>1.09</v>
@@ -4328,7 +4328,7 @@
         <v>8971</v>
       </c>
       <c r="B150" t="n">
-        <v>36729.90816281663</v>
+        <v>36729.90816281664</v>
       </c>
       <c r="C150" t="n">
         <v>1.09</v>
@@ -4354,7 +4354,7 @@
         <v>8972</v>
       </c>
       <c r="B151" t="n">
-        <v>25183.06960250684</v>
+        <v>25183.06960250685</v>
       </c>
       <c r="C151" t="n">
         <v>1.09</v>
@@ -4406,7 +4406,7 @@
         <v>8974</v>
       </c>
       <c r="B153" t="n">
-        <v>34829.09958970878</v>
+        <v>34829.09958970874</v>
       </c>
       <c r="C153" t="n">
         <v>1.09</v>
@@ -4536,7 +4536,7 @@
         <v>8979</v>
       </c>
       <c r="B158" t="n">
-        <v>25601.04394475286</v>
+        <v>25601.04394475287</v>
       </c>
       <c r="C158" t="n">
         <v>1.09</v>

</xml_diff>